<commit_message>
add the game info of the greedy family
Signed-off-by: oohju <zhaoyujia007@gmail.com>
</commit_message>
<xml_diff>
--- a/documents/timeManage/TimeManage_ZYJ.xlsx
+++ b/documents/timeManage/TimeManage_ZYJ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>日期</t>
   </si>
@@ -84,6 +84,14 @@
   </si>
   <si>
     <t>设计游戏《可爱糖果对对碰》思路，并上传</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.4.16</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据周日的讨论，重新设计《贪食家族》游戏，并上传</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -454,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -553,6 +561,17 @@
       </c>
       <c r="D7">
         <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="27">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update time manage document
Signed-off-by: oohju <zhaoyujia007@gmail.com>
</commit_message>
<xml_diff>
--- a/documents/timeManage/TimeManage_ZYJ.xlsx
+++ b/documents/timeManage/TimeManage_ZYJ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>日期</t>
   </si>
@@ -145,6 +145,39 @@
   </si>
   <si>
     <t>调试代码发现触摸层不能被自动释放，加入触摸层的pause，bag相关代码</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.4.25</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>将新素材加入纹理图</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.4.26</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.4.27</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>初步完成飞行动物的动画</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>场景切换，body释放会段错，现在暂时没有释放。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>精灵在entity里申明的，显示不出来，必须要在子类再次申明一下。没明白为什么。
+飞行动物碰撞边框后，方向有点错误</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.加入飞行动画。2.调试场景切换bug，未成功。3.修改一处操作，要先触摸到飞行动物才能移动。</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -521,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -694,6 +727,45 @@
       </c>
       <c r="D13">
         <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="40.5">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="40.5">
+      <c r="A16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update bag and propert ball
Signed-off-by: oohju <zhaoyujia007@gmail.com>
</commit_message>
<xml_diff>
--- a/documents/timeManage/TimeManage_ZYJ.xlsx
+++ b/documents/timeManage/TimeManage_ZYJ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>日期</t>
   </si>
@@ -198,6 +198,22 @@
   </si>
   <si>
     <t>动作添加了，但是没有显示出来</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.5.4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>加入属性球，和背包触摸控制</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.5.5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>用menu类为背包添加图像</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -574,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -810,6 +826,28 @@
         <v>45</v>
       </c>
       <c r="D18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modify the move style
Signed-off-by: oohju <zhaoyujia007@gmail.com>
</commit_message>
<xml_diff>
--- a/documents/timeManage/TimeManage_ZYJ.xlsx
+++ b/documents/timeManage/TimeManage_ZYJ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>日期</t>
   </si>
@@ -242,6 +242,34 @@
   </si>
   <si>
     <t>从下落，到得分，已经基本调通</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>研究通知模块</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要开发者账户</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>设计关卡，调试</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>关卡调试，糖果运行轨迹调试</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.6.5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.6.6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.6.7</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -618,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -913,6 +941,42 @@
       </c>
       <c r="D23">
         <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add cover of the candy And modify the way of del ball
Signed-off-by: oohju <zhaoyujia007@gmail.com>
</commit_message>
<xml_diff>
--- a/documents/timeManage/TimeManage_ZYJ.xlsx
+++ b/documents/timeManage/TimeManage_ZYJ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>日期</t>
   </si>
@@ -270,6 +270,58 @@
   </si>
   <si>
     <t>2012.6.7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.6.17</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据设计，代码修改实现20关</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>20关卡设计</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>小组会议</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.小鸟控制修改：改为手势控制；2消分判断修改：仓库最后3个一样才能触发消分。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>消分时现在是从左到右遍历，需要改为从右向左遍历</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.6.15</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.6.14</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>碰撞后糖果运行轨迹还需要更好的算法</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>后续可以加入包装的糖果</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.6.10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.6.21</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>加入包装糖果，修改消分时从右往左遍历</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -646,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -975,8 +1027,69 @@
       <c r="B26" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="C26" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="D26">
         <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="27">
+      <c r="A27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31">
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update time doc and xcodeproj
Signed-off-by: oohju <zhaoyujia007@gmail.com>
</commit_message>
<xml_diff>
--- a/documents/timeManage/TimeManage_ZYJ.xlsx
+++ b/documents/timeManage/TimeManage_ZYJ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>日期</t>
   </si>
@@ -362,6 +362,14 @@
   </si>
   <si>
     <t>修改撞墙后下落方向， 添加动画</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.6.28</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改一处属性球bug，判断球回收为hitpoint为-1</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -738,9 +746,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
@@ -1180,6 +1188,17 @@
       </c>
       <c r="D35">
         <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="27">
+      <c r="A36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify prop architecture. fix out some bugs. add increase and decrease ball
Signed-off-by: oohju <zhaoyujia007@gmail.com>
</commit_message>
<xml_diff>
--- a/documents/timeManage/TimeManage_ZYJ.xlsx
+++ b/documents/timeManage/TimeManage_ZYJ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="106">
   <si>
     <t>日期</t>
   </si>
@@ -430,6 +430,14 @@
   </si>
   <si>
     <t>修改落地方向 和 弹力过大bug</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.7.16</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>调整 prop代码，加入加速 减速属性球。</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -806,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1347,6 +1355,17 @@
       </c>
       <c r="D44">
         <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D45">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reduce flay animate to 2 directs; add some storage action
Signed-off-by: oohju <zhaoyujia007@gmail.com>
</commit_message>
<xml_diff>
--- a/documents/timeManage/TimeManage_ZYJ.xlsx
+++ b/documents/timeManage/TimeManage_ZYJ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="121">
   <si>
     <t>日期</t>
   </si>
@@ -462,6 +462,44 @@
   </si>
   <si>
     <t>研究特效。初步加入气球破裂和球落地特效</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>加入动物中属性球特效  加入小猪</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.7.20</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.7.21</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>小组会议</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.7.22</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>把飞行动物动画减少为2个方向。添加一些仓库
+action</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>飞行动物动画需要精细化处理。比如眨眼，蹬腿。
+和随着飞行速度改变翅膀频率。动画像素改变方法还没找到</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>特效效果需要再调。 得分特效还没找到怎么做</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>亲历北京有史以来最大暴雨</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -838,10 +876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1423,6 +1461,45 @@
       </c>
       <c r="D48">
         <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D49">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="40.5">
+      <c r="A51" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D51">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1.add dropped things dispear action 2.add fly animation speed transform
Signed-off-by: oohju <zhaoyujia007@gmail.com>
</commit_message>
<xml_diff>
--- a/documents/timeManage/TimeManage_ZYJ.xlsx
+++ b/documents/timeManage/TimeManage_ZYJ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="124">
   <si>
     <t>日期</t>
   </si>
@@ -500,6 +500,19 @@
   </si>
   <si>
     <t>亲历北京有史以来最大暴雨</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.7.22</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>加入根据飞行速度调节翅膀频率。加入落地
+物品消失action</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>水晶球削球有bug。未找出</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -876,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1500,6 +1513,20 @@
       </c>
       <c r="D51">
         <v>2.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="27">
+      <c r="A52" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change the method of the way when the storage is full.
Signed-off-by: oohju <zhaoyujia007@gmail.com>
</commit_message>
<xml_diff>
--- a/documents/timeManage/TimeManage_ZYJ.xlsx
+++ b/documents/timeManage/TimeManage_ZYJ.xlsx
@@ -508,11 +508,12 @@
   </si>
   <si>
     <t>加入根据飞行速度调节翅膀频率。加入落地
-物品消失action</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>水晶球削球有bug。未找出</t>
+物品消失action。仓库满时，改为把第一个挤掉</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>水晶球削球好像有bug。未找出。看代码没看出来
+仓库削球效果没有层次感</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -892,7 +893,7 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1515,18 +1516,18 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="27">
+    <row r="52" spans="1:4" ht="40.5">
       <c r="A52" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="2" t="s">
         <v>123</v>
       </c>
       <c r="D52">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add some spc when storage  del the ball and when fly speed is fast
Signed-off-by: oohju <zhaoyujia007@gmail.com>
</commit_message>
<xml_diff>
--- a/documents/timeManage/TimeManage_ZYJ.xlsx
+++ b/documents/timeManage/TimeManage_ZYJ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="131">
   <si>
     <t>日期</t>
   </si>
@@ -522,6 +522,26 @@
   </si>
   <si>
     <t>加入剩余球计数；调整动画；手机设置图标</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.7.24</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>加入每次得分显示，以及特效</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>效果不是很满意，特别是特效</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.7.25</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>加入削球特效。和飞行动物速度达到一定时特效效果一般</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -898,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1547,6 +1567,31 @@
       </c>
       <c r="D53">
         <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D55">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add leaderboard and archievements
Signed-off-by: oohju <zhaoyujia007@gmail.com>
</commit_message>
<xml_diff>
--- a/documents/timeManage/TimeManage_ZYJ.xlsx
+++ b/documents/timeManage/TimeManage_ZYJ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="133">
   <si>
     <t>日期</t>
   </si>
@@ -542,6 +542,14 @@
   </si>
   <si>
     <t>加入削球特效。和飞行动物速度达到一定时特效效果一般</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.7.28+29</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加game center的排行榜和成就</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -918,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1592,6 +1600,17 @@
       </c>
       <c r="D55">
         <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D56">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix a save bug
Signed-off-by: oohju <zhaoyujia007@gmail.com>
</commit_message>
<xml_diff>
--- a/documents/timeManage/TimeManage_ZYJ.xlsx
+++ b/documents/timeManage/TimeManage_ZYJ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="138">
   <si>
     <t>日期</t>
   </si>
@@ -550,6 +550,26 @@
   </si>
   <si>
     <t>增加game center的排行榜和成就</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.7.30</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加较色切换  累计得分</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.7.31+8.1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加商店</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>存储数据老被清0.或读错。是不是没有初始化？</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -926,10 +946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1611,6 +1631,31 @@
       </c>
       <c r="D56">
         <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D58">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update time mark, update a log pic
Signed-off-by: oohju <zhaoyujia007@gmail.com>
</commit_message>
<xml_diff>
--- a/documents/timeManage/TimeManage_ZYJ.xlsx
+++ b/documents/timeManage/TimeManage_ZYJ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="179">
   <si>
     <t>日期</t>
   </si>
@@ -646,6 +646,95 @@
   </si>
   <si>
     <t xml:space="preserve">添加属性球 包装   </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>小组会议</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改loading界面 初步制作教学图片</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>制作 开发者展示界面</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>界面风格不统一</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>教学界面需要调整</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.8.9.5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.8.9.9</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.8.9.16</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.8.9.22</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.8.9.20</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成暂停时教学界面，调整暂停界面摆设</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成开始弹出教学界面;初步制作暂停时教学界面;调整商店等图标</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>调整奖励，出属性球策略</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加熊猫</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改纹理图</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.10.23</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.10.24</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加仓库可用和不可用</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>整理z轴</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.11.3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.11.4</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1022,10 +1111,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1833,6 +1922,116 @@
         <v>153</v>
       </c>
       <c r="D67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D70">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="27">
+      <c r="A71" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D71">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D72">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="B73" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D74">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D77">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modify progress add some music
Signed-off-by: oohju <zhaoyujia007@gmail.com>
</commit_message>
<xml_diff>
--- a/documents/timeManage/TimeManage_ZYJ.xlsx
+++ b/documents/timeManage/TimeManage_ZYJ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="198">
   <si>
     <t>日期</t>
   </si>
@@ -787,6 +787,30 @@
   </si>
   <si>
     <t>load game添加 教学图片</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.11.25</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>代码结构重构，ipad同步</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.12.2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>结束界面，字体，特效，</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>刘云鹏，赵羽佳，刘晋 集中开发</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色进度条修改</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1163,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" topLeftCell="B67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2149,6 +2173,39 @@
       </c>
       <c r="D82">
         <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D84">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="B85" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D85">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify the load teach  display layer
Signed-off-by: oohju <zhaoyujia007@gmail.com>
</commit_message>
<xml_diff>
--- a/documents/timeManage/TimeManage_ZYJ.xlsx
+++ b/documents/timeManage/TimeManage_ZYJ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="203">
   <si>
     <t>日期</t>
   </si>
@@ -811,6 +811,26 @@
   </si>
   <si>
     <t>角色进度条修改</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.12.8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.12.4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改开始界面特效</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.12.9</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改loading界面 教学 和 展示  修改奶酪下落轨迹</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1187,10 +1207,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" topLeftCell="C67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F85" sqref="F85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2201,11 +2221,36 @@
       </c>
     </row>
     <row r="85" spans="1:4">
+      <c r="A85" s="1" t="s">
+        <v>199</v>
+      </c>
       <c r="B85" s="1" t="s">
         <v>197</v>
       </c>
       <c r="D85">
         <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D87">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>